<commit_message>
updated leveled games to insure minimal gap is tried. added functionality of comparing session rounds
</commit_message>
<xml_diff>
--- a/4_Niveau.xlsx
+++ b/4_Niveau.xlsx
@@ -217,9 +217,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10.0"/>
@@ -359,22 +356,22 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1351,16 +1348,17 @@
       <c r="B32" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="11">
         <f>ROUND(AVERAGE('Form Responses 1'!$D32:$G32),1)</f>
         <v>2</v>
       </c>
-      <c r="D32" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="C33" s="19"/>

</xml_diff>